<commit_message>
Update documentation of each testcases : Service Layer Fixes #126
</commit_message>
<xml_diff>
--- a/testing/OperationKeyManagement+testcase.docs.xlsx
+++ b/testing/OperationKeyManagement+testcase.docs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venka\Documents\MW\OKM\12_04_23\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venka\Documents\GitHub\Test2\OperationKeyManagement\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E0D34A-7514-498A-A2A0-73B22E4BEDD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E1A881-151C-4DA0-ABCB-F647DE91BB60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{8A4BF7CC-909B-4C1B-B59F-29AF2D960B3A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="224">
   <si>
     <t>Testcases</t>
   </si>
@@ -484,10 +484,6 @@
     <t>##Gets new-application-address update trigger update-ltp to ALT?</t>
   </si>
   <si>
-    <t>#### Clearance check:
-- Check if the logical-termination-point instance is the same as initial configuration</t>
-  </si>
-  <si>
     <t>##Gets new-application-port update trigger update-ltp to ALT?</t>
   </si>
   <si>
@@ -1130,27 +1126,6 @@
   </si>
   <si>
     <t>#### Testing:
-- POST ExecutionAndTraceLog/v1/list-records-of-flow with 
-   - IP and port from above
-   - operation-key from above
-   - DummyValue of x-correlator
-   - checking response 
-   - checking same record for containing DummyXCorrelator and 
-each callback is present .
-POST - 3 min - eatl log -x-core - check entries
-timer 10 min - loop for every 1 min, to check if last forwarding is executed/not</t>
-  </si>
-  <si>
-    <t>#### Testing:
-- POST ExecutionAndTraceLog/v1/list-records-of-flow with 
-   - IP and port from above
-   - operation-key from above
-   - DummyValue of x-correlator
-   - checking response for entry with application data from ServiceRequestCausesLtpUpdateRequest
-   - checking same record for containing DummyXCorrelator &amp;DummyTraceIndicator</t>
-  </si>
-  <si>
-    <t>#### Testing:
 - checking for ResponseCode==204
 - GETing CC (/core-model-1-4:control-construct)
 - verify that CC/http-c application-name=dummyApplicationName and its corresponding release-number</t>
@@ -1168,24 +1143,6 @@
   - dummy values generated for application-name, release-number, address, port, port 
    -operation-key from above
    - reasonable parameter</t>
-  </si>
-  <si>
-    <t>#### Testing:
-- POST ExecutionAndTraceLog/v1/list-records-of-flow with 
-   - IP and port from above
-   - operation-key from above
-   - DummyValue of x-correlator
-   - checking response for entry with application data from ServiceRequestCausesFcUpdateRequest
-   - checking same record for containing DummyXCorrelator &amp;DummyTraceIndicator</t>
-  </si>
-  <si>
-    <t>#### Testing:
-- POST ExecutionAndTraceLog/v1/list-records-of-flow with 
-   - IP and port from above
-   - operation-key from above
-   - DummyValue of x-correlator
-   - checking response for entry with application data from ServiceRequestCausesLtpDeletionRequest
-   - checking same record for containing DummyXCorrelator &amp;DummyTraceIndicator</t>
   </si>
   <si>
     <t>#### Preparation:
@@ -1263,26 +1220,6 @@
 - ApplicationLayerTopology server to operate</t>
   </si>
   <si>
-    <t>#### Preparation:
-- GETing CC (/core-model-1-4:control-construct)
-  - search CC for output fc-port of ServiceRequestCausesLoggingRequest, 
-its corresponding op-c, http-c and tcp-c, storing them for later verification request
-  - searching CC for output-fc-port of ServiceRequestCausesLtpUpdateRequest, its corresponding op-c, http-c, storing them.
-  - searching CC for output-fc-port of CyclicOperationCausesRequestForListOfLinks, its corresponding op-c, storing them.
-  - searching CC for output-fc-port of CyclicOperationCausesRequestForLinkEndPoints, its corresponding op-c, storing them.
-   - searching CC for op-s of /v1/regard-updated-link storing operation-key
-- GETting EaTL/CC (while using IP and port from above)
-   - searching CC for op-c of /v1/list-records-of-flow, storing operation-key
-- POST ALT/v1/list-link-uuids - For getting link-uuid
-  - randonly select a link-uuid and store it
-- POST ALT/v1/list-end-points-of-link - For getting link end points
- - extract Link End Point list from response-body and store it 
-- POST /v1/regard-updated-link with  
-   - attribute according to randomly chosen link-uuid from above
-   -operation-key from above
-   - all parameters with realistic values (incl. DummyXCorrelator)</t>
-  </si>
-  <si>
     <t>#### Testing:
 - POST ExecutionAndTraceLog/v1/list-records-of-flow with 
    - IP, protocol and port from above
@@ -1390,6 +1327,65 @@
 - checking for ResponseCode==204
 - GETing CC (/core-model-1-4:control-construct)
   - searching for forwarding-construct of   LinkUpdateNotificationCausesOperationKeyUpdates and CyclicOperationCausesOperationKeyUpdates with logical-termination-point and verify that fc port present for dummy created application</t>
+  </si>
+  <si>
+    <t>#### Testing:
+- POST ExecutionAndTraceLog/v1/list-records-of-flow with 
+   - IP, protocol and port from above
+   - operation-key from above
+   - DummyValue of x-correlator
+   - checking response for entry with application data from ServiceRequestCausesLtpUpdateRequest
+   - checking same record for containing DummyXCorrelator &amp;DummyTraceIndicator</t>
+  </si>
+  <si>
+    <t>#### Testing:
+- POST ExecutionAndTraceLog/v1/list-records-of-flow with 
+   - IP, protocol and port from above
+   - operation-key from above
+   - DummyValue of x-correlator
+   - checking response for entry with application data from ServiceRequestCausesLtpDeletionRequest
+   - checking same record for containing DummyXCorrelator &amp;DummyTraceIndicator</t>
+  </si>
+  <si>
+    <t>#### Testing:
+- POST ExecutionAndTraceLog/v1/list-records-of-flow with 
+   - IP, protocol and port from above
+   - operation-key from above
+   - DummyValue of x-correlator
+   - checking response for entry with application data from ServiceRequestCausesFcUpdateRequest
+   - checking same record for containing DummyXCorrelator &amp;DummyTraceIndicator</t>
+  </si>
+  <si>
+    <t>#### Testing:
+- POST ExecutionAndTraceLog/v1/list-records-of-flow with 
+   - IP, protocol and port from above
+   - operation-key from above
+   - DummyValue of x-correlator
+   - checking response 
+   - checking same record for containing DummyXCorrelator and 
+each callback is present .
+POST - 3 min - eatl log -x-core - check entries
+timer 10 min - loop for every 1 min, to check if last forwarding is executed/not</t>
+  </si>
+  <si>
+    <t>#### Preparation:
+- GETing CC (/core-model-1-4:control-construct)
+  - search CC for output fc-port of ServiceRequestCausesLoggingRequest, 
+its corresponding op-c, http-c and tcp-c, storing them for later verification request
+  - searching CC for output-fc-port of ServiceRequestCausesLtpUpdateRequest, its corresponding op-c, http-c, storing them.
+  - searching CC for output-fc-port of CyclicOperationCausesRequestForListOfLinks, its corresponding op-c, storing them.
+  - searching CC for output-fc-port of CyclicOperationCausesRequestForLinkEndPoints, its corresponding op-c, storing them.
+   - searching CC for op-s of /v1/regard-updated-link storing operation-key
+- GETting EaTL/CC (while using IP, protocol and port from above)
+   - searching CC for op-c of /v1/list-records-of-flow, storing operation-key
+- POST ALT/v1/list-link-uuids - For getting link-uuid
+  - randonly select a link-uuid and store it
+- POST ALT/v1/list-end-points-of-link - For getting link end points
+ - extract Link End Point list from response-body and store it 
+- POST /v1/regard-updated-link with  
+   - attribute according to randomly chosen link-uuid from above
+   -operation-key from above
+   - all parameters with realistic values (incl. DummyXCorrelator)</t>
   </si>
 </sst>
 </file>
@@ -1851,6 +1847,13 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1859,13 +1862,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2186,10 +2182,10 @@
   <dimension ref="A1:G223"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="C167" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B147" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E123" sqref="E123"/>
+      <selection pane="bottomRight" activeCell="D150" sqref="D150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2204,7 +2200,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A1" s="54" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="17"/>
@@ -2245,11 +2241,11 @@
         <v>88</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="62" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -2277,12 +2273,12 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="59"/>
+      <c r="A5" s="62"/>
       <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D5" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -2356,7 +2352,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="59"/>
+      <c r="A6" s="62"/>
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
@@ -2391,12 +2387,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A7" s="59"/>
+      <c r="A7" s="62"/>
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D7" s="23" t="str">
         <f>$B7</f>
@@ -2420,7 +2416,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="62" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -2448,12 +2444,12 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="59"/>
+      <c r="A9" s="62"/>
       <c r="B9" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D9" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -2527,7 +2523,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="59"/>
+      <c r="A10" s="62"/>
       <c r="B10" s="8" t="s">
         <v>11</v>
       </c>
@@ -2558,14 +2554,14 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A11" s="59"/>
+      <c r="A11" s="62"/>
       <c r="B11" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D11" s="26" t="str">
         <f>$B7</f>
@@ -2589,7 +2585,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="59" t="s">
+      <c r="A12" s="62" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -2617,12 +2613,12 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="203" x14ac:dyDescent="0.35">
-      <c r="A13" s="59"/>
+      <c r="A13" s="62"/>
       <c r="B13" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D13" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -2697,7 +2693,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="59"/>
+      <c r="A14" s="62"/>
       <c r="B14" s="8" t="s">
         <v>15</v>
       </c>
@@ -2728,14 +2724,14 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A15" s="59"/>
+      <c r="A15" s="62"/>
       <c r="B15" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D15" s="23" t="str">
         <f>$B7</f>
@@ -2759,7 +2755,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="59" t="s">
+      <c r="A16" s="62" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -2787,12 +2783,12 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="203" x14ac:dyDescent="0.35">
-      <c r="A17" s="59"/>
+      <c r="A17" s="62"/>
       <c r="B17" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D17" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -2865,7 +2861,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="59"/>
+      <c r="A18" s="62"/>
       <c r="B18" s="8" t="s">
         <v>15</v>
       </c>
@@ -2896,14 +2892,14 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A19" s="59"/>
+      <c r="A19" s="62"/>
       <c r="B19" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D19" s="30" t="str">
         <f>$B7</f>
@@ -2927,7 +2923,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="59" t="s">
+      <c r="A20" s="62" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -2955,12 +2951,12 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="203" x14ac:dyDescent="0.35">
-      <c r="A21" s="59"/>
+      <c r="A21" s="62"/>
       <c r="B21" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D21" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -3033,7 +3029,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="59"/>
+      <c r="A22" s="62"/>
       <c r="B22" s="8" t="s">
         <v>15</v>
       </c>
@@ -3064,14 +3060,14 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A23" s="59"/>
+      <c r="A23" s="62"/>
       <c r="B23" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D23" s="30" t="str">
         <f>$B7</f>
@@ -3095,7 +3091,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="59" t="s">
+      <c r="A24" s="62" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -3123,12 +3119,12 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="59"/>
+      <c r="A25" s="62"/>
       <c r="B25" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D25" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -3186,7 +3182,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="59"/>
+      <c r="A26" s="62"/>
       <c r="B26" s="8" t="s">
         <v>25</v>
       </c>
@@ -3217,14 +3213,14 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="59"/>
+      <c r="A27" s="62"/>
       <c r="B27" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D27" s="23" t="str">
         <f>$B7</f>
@@ -3248,7 +3244,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="59" t="s">
+      <c r="A28" s="62" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="7" t="s">
@@ -3276,12 +3272,12 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="59"/>
+      <c r="A29" s="62"/>
       <c r="B29" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D29" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -3339,7 +3335,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="59"/>
+      <c r="A30" s="62"/>
       <c r="B30" s="8" t="s">
         <v>25</v>
       </c>
@@ -3370,14 +3366,14 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A31" s="59"/>
+      <c r="A31" s="62"/>
       <c r="B31" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D31" s="23" t="str">
         <f>$B7</f>
@@ -3401,7 +3397,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="59" t="s">
+      <c r="A32" s="62" t="s">
         <v>29</v>
       </c>
       <c r="B32" s="7" t="s">
@@ -3429,7 +3425,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="59"/>
+      <c r="A33" s="62"/>
       <c r="B33" s="8" t="s">
         <v>31</v>
       </c>
@@ -3487,12 +3483,12 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A34" s="59"/>
+      <c r="A34" s="62"/>
       <c r="B34" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C34" s="48" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D34" s="29" t="str">
         <f>$C34</f>
@@ -3507,21 +3503,21 @@
 - checking for ResponseHeaders (x-correlator, exec-time, backend-time and life-cycle-state) being present and checking for correctness of type of each parameter.</v>
       </c>
       <c r="F34" s="48" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G34" s="48" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A35" s="59"/>
+      <c r="A35" s="62"/>
       <c r="B35" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D35" s="30" t="str">
         <f>$B7</f>
@@ -3545,7 +3541,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="59" t="s">
+      <c r="A36" s="62" t="s">
         <v>33</v>
       </c>
       <c r="B36" s="7" t="s">
@@ -3573,7 +3569,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="59"/>
+      <c r="A37" s="62"/>
       <c r="B37" s="8" t="s">
         <v>31</v>
       </c>
@@ -3631,7 +3627,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="59"/>
+      <c r="A38" s="62"/>
       <c r="B38" s="8" t="s">
         <v>35</v>
       </c>
@@ -3654,21 +3650,21 @@
 - checking for response headers containing x-correlator==dummyXCorrelator</v>
       </c>
       <c r="F38" s="48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G38" s="48" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A39" s="59"/>
+      <c r="A39" s="62"/>
       <c r="B39" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D39" s="23" t="str">
         <f>$B7</f>
@@ -3692,7 +3688,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="59" t="s">
+      <c r="A40" s="62" t="s">
         <v>36</v>
       </c>
       <c r="B40" s="7" t="s">
@@ -3720,7 +3716,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="60"/>
+      <c r="A41" s="63"/>
       <c r="B41" s="8" t="s">
         <v>31</v>
       </c>
@@ -3778,7 +3774,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="60"/>
+      <c r="A42" s="63"/>
       <c r="B42" s="8" t="s">
         <v>38</v>
       </c>
@@ -3824,14 +3820,14 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A43" s="60"/>
+      <c r="A43" s="63"/>
       <c r="B43" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D43" s="23" t="str">
         <f>$B7</f>
@@ -3855,7 +3851,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="59" t="s">
+      <c r="A44" s="62" t="s">
         <v>39</v>
       </c>
       <c r="B44" s="7" t="s">
@@ -3878,7 +3874,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="60"/>
+      <c r="A45" s="63"/>
       <c r="B45" s="8" t="s">
         <v>41</v>
       </c>
@@ -3899,12 +3895,12 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="246.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="60"/>
+      <c r="A46" s="63"/>
       <c r="B46" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D46" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -4010,9 +4006,9 @@
       </c>
     </row>
     <row r="47" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="60"/>
+      <c r="A47" s="63"/>
       <c r="B47" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C47" s="29" t="str">
         <f>CONCATENATE("#### Testing:
@@ -4096,14 +4092,14 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="60"/>
+      <c r="A48" s="63"/>
       <c r="B48" s="9" t="str">
         <f>$B7</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
       <c r="C48" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D48" s="32" t="str">
         <f>$B7</f>
@@ -4138,7 +4134,7 @@
       <c r="G49" s="3"/>
     </row>
     <row r="50" spans="1:7" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="61" t="s">
+      <c r="A50" s="64" t="s">
         <v>43</v>
       </c>
       <c r="B50" s="11" t="s">
@@ -4157,11 +4153,11 @@
         <v>44</v>
       </c>
       <c r="G50" s="34" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="87" x14ac:dyDescent="0.35">
-      <c r="A51" s="59"/>
+      <c r="A51" s="62"/>
       <c r="B51" s="12" t="s">
         <v>45</v>
       </c>
@@ -4193,7 +4189,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="171" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="59"/>
+      <c r="A52" s="62"/>
       <c r="B52" s="13" t="s">
         <v>46</v>
       </c>
@@ -4207,12 +4203,12 @@
         <v>90</v>
       </c>
       <c r="F52" s="51" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G52" s="51"/>
     </row>
     <row r="53" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A53" s="59"/>
+      <c r="A53" s="62"/>
       <c r="B53" s="14" t="s">
         <v>47</v>
       </c>
@@ -4233,7 +4229,7 @@
       <c r="G53" s="37"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A54" s="60" t="s">
+      <c r="A54" s="63" t="s">
         <v>48</v>
       </c>
       <c r="B54" s="11" t="s">
@@ -4256,7 +4252,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" ht="174" x14ac:dyDescent="0.35">
-      <c r="A55" s="60"/>
+      <c r="A55" s="63"/>
       <c r="B55" s="12" t="s">
         <v>50</v>
       </c>
@@ -4298,7 +4294,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A56" s="60"/>
+      <c r="A56" s="63"/>
       <c r="B56" s="13" t="s">
         <v>51</v>
       </c>
@@ -4319,7 +4315,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A57" s="60"/>
+      <c r="A57" s="63"/>
       <c r="B57" s="14" t="s">
         <v>47</v>
       </c>
@@ -4340,7 +4336,7 @@
       </c>
     </row>
     <row r="58" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A58" s="60"/>
+      <c r="A58" s="63"/>
       <c r="B58" s="13" t="s">
         <v>52</v>
       </c>
@@ -4352,14 +4348,14 @@
         <v>90</v>
       </c>
       <c r="F58" s="24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G58" s="52" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A59" s="59" t="s">
+      <c r="A59" s="62" t="s">
         <v>53</v>
       </c>
       <c r="B59" s="7" t="s">
@@ -4387,12 +4383,12 @@
       </c>
     </row>
     <row r="60" spans="1:7" ht="203" x14ac:dyDescent="0.35">
-      <c r="A60" s="60"/>
+      <c r="A60" s="63"/>
       <c r="B60" s="8" t="s">
         <v>55</v>
       </c>
       <c r="C60" s="21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D60" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -4472,7 +4468,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A61" s="60"/>
+      <c r="A61" s="63"/>
       <c r="B61" s="8" t="s">
         <v>56</v>
       </c>
@@ -4493,12 +4489,12 @@
       </c>
     </row>
     <row r="62" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="60"/>
+      <c r="A62" s="63"/>
       <c r="B62" s="15" t="s">
         <v>57</v>
       </c>
       <c r="C62" s="38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D62" s="38" t="s">
         <v>57</v>
@@ -4514,7 +4510,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A63" s="59" t="s">
+      <c r="A63" s="62" t="s">
         <v>58</v>
       </c>
       <c r="B63" s="7" t="s">
@@ -4542,12 +4538,12 @@
       </c>
     </row>
     <row r="64" spans="1:7" ht="203" x14ac:dyDescent="0.35">
-      <c r="A64" s="59"/>
+      <c r="A64" s="62"/>
       <c r="B64" s="8" t="s">
         <v>60</v>
       </c>
       <c r="C64" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D64" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -4589,11 +4585,11 @@
         <v>90</v>
       </c>
       <c r="G64" s="21" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A65" s="59"/>
+      <c r="A65" s="62"/>
       <c r="B65" s="8" t="s">
         <v>61</v>
       </c>
@@ -4622,7 +4618,7 @@
       </c>
     </row>
     <row r="66" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="59"/>
+      <c r="A66" s="62"/>
       <c r="B66" s="15" t="s">
         <v>47</v>
       </c>
@@ -4651,8 +4647,8 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A67" s="59" t="s">
-        <v>134</v>
+      <c r="A67" s="62" t="s">
+        <v>133</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>62</v>
@@ -4679,7 +4675,7 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A68" s="59"/>
+      <c r="A68" s="62"/>
       <c r="B68" s="8"/>
       <c r="C68" s="41" t="s">
         <v>94</v>
@@ -4688,20 +4684,20 @@
         <v>93</v>
       </c>
       <c r="E68" s="41" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F68" s="39" t="s">
         <v>90</v>
       </c>
       <c r="G68" s="41" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="203" x14ac:dyDescent="0.35">
-      <c r="A69" s="59"/>
+      <c r="A69" s="62"/>
       <c r="B69" s="8"/>
       <c r="C69" s="21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D69" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -4733,11 +4729,11 @@
     - reasonable parameters but release-number attribute with random dummy value (that doesnot comply specification</v>
       </c>
       <c r="G69" s="21" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A70" s="59"/>
+      <c r="A70" s="62"/>
       <c r="B70" s="8"/>
       <c r="C70" s="25" t="str">
         <f ca="1">$C70</f>
@@ -4755,7 +4751,7 @@
       </c>
     </row>
     <row r="71" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A71" s="59"/>
+      <c r="A71" s="62"/>
       <c r="B71" s="8"/>
       <c r="C71" s="22" t="str">
         <f>$B15</f>
@@ -4779,23 +4775,23 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A72" s="59"/>
+      <c r="A72" s="62"/>
       <c r="B72" s="8"/>
       <c r="C72" s="41" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D72" s="41" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G72" s="41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="203" x14ac:dyDescent="0.35">
-      <c r="A73" s="59"/>
+      <c r="A73" s="62"/>
       <c r="B73" s="8"/>
       <c r="C73" s="21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D73" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -4819,7 +4815,7 @@
       <c r="G73" s="21"/>
     </row>
     <row r="74" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A74" s="59"/>
+      <c r="A74" s="62"/>
       <c r="B74" s="8"/>
       <c r="C74" s="25" t="str">
         <f ca="1">$C74</f>
@@ -4834,7 +4830,7 @@
       <c r="G74" s="25"/>
     </row>
     <row r="75" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A75" s="59"/>
+      <c r="A75" s="62"/>
       <c r="B75" s="8"/>
       <c r="C75" s="50" t="str">
         <f t="shared" ref="C75" si="0">$B35</f>
@@ -4849,20 +4845,20 @@
       <c r="G75" s="22"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A76" s="59"/>
+      <c r="A76" s="62"/>
       <c r="B76" s="8"/>
       <c r="C76" s="41" t="s">
         <v>95</v>
       </c>
       <c r="D76" s="41" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="203" x14ac:dyDescent="0.35">
-      <c r="A77" s="59"/>
+      <c r="A77" s="62"/>
       <c r="B77" s="8"/>
       <c r="C77" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D77" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -4885,7 +4881,7 @@
       </c>
     </row>
     <row r="78" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A78" s="59"/>
+      <c r="A78" s="62"/>
       <c r="B78" s="8"/>
       <c r="C78" s="25" t="str">
         <f ca="1">$C78</f>
@@ -4899,7 +4895,7 @@
       </c>
     </row>
     <row r="79" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A79" s="59"/>
+      <c r="A79" s="62"/>
       <c r="B79" s="8"/>
       <c r="C79" s="22" t="str">
         <f>$B15</f>
@@ -4913,20 +4909,20 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A80" s="59"/>
+      <c r="A80" s="62"/>
       <c r="B80" s="8"/>
       <c r="C80" s="41" t="s">
         <v>96</v>
       </c>
       <c r="D80" s="41" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="203" x14ac:dyDescent="0.35">
-      <c r="A81" s="59"/>
+      <c r="A81" s="62"/>
       <c r="B81" s="8"/>
       <c r="C81" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D81" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -4949,7 +4945,7 @@
       </c>
     </row>
     <row r="82" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A82" s="59"/>
+      <c r="A82" s="62"/>
       <c r="B82" s="8"/>
       <c r="C82" s="25" t="str">
         <f ca="1">$C82</f>
@@ -4963,7 +4959,7 @@
       </c>
     </row>
     <row r="83" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A83" s="59"/>
+      <c r="A83" s="62"/>
       <c r="B83" s="8"/>
       <c r="C83" s="22" t="str">
         <f>$B19</f>
@@ -4977,15 +4973,15 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A84" s="59"/>
+      <c r="A84" s="62"/>
       <c r="B84" s="8"/>
       <c r="C84" s="22"/>
       <c r="D84" s="41" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A85" s="59"/>
+      <c r="A85" s="62"/>
       <c r="B85" s="8"/>
       <c r="C85" s="22"/>
       <c r="D85" s="21" t="str">
@@ -5009,7 +5005,7 @@
       </c>
     </row>
     <row r="86" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A86" s="59"/>
+      <c r="A86" s="62"/>
       <c r="B86" s="8"/>
       <c r="C86" s="22"/>
       <c r="D86" s="25" t="str">
@@ -5019,7 +5015,7 @@
       </c>
     </row>
     <row r="87" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A87" s="59"/>
+      <c r="A87" s="62"/>
       <c r="B87" s="8"/>
       <c r="C87" s="22"/>
       <c r="D87" s="22" t="str">
@@ -5029,7 +5025,7 @@
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A88" s="59" t="s">
+      <c r="A88" s="62" t="s">
         <v>63</v>
       </c>
       <c r="B88" s="7" t="s">
@@ -5057,10 +5053,10 @@
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A89" s="59"/>
+      <c r="A89" s="62"/>
       <c r="B89" s="8"/>
       <c r="C89" s="41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D89" s="41" t="s">
         <v>98</v>
@@ -5074,18 +5070,18 @@
       <c r="G89" s="41"/>
     </row>
     <row r="90" spans="1:7" ht="303" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="60"/>
+      <c r="A90" s="63"/>
       <c r="B90" s="8" t="s">
         <v>65</v>
       </c>
       <c r="C90" s="21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D90" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E90" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F90" s="52" t="s">
         <v>90</v>
@@ -5095,31 +5091,31 @@
       </c>
     </row>
     <row r="91" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="60"/>
+      <c r="A91" s="63"/>
       <c r="B91" s="8" t="s">
         <v>66</v>
       </c>
       <c r="C91" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="D91" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="E91" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="D91" s="25" t="s">
-        <v>198</v>
-      </c>
-      <c r="E91" s="25" t="s">
-        <v>173</v>
-      </c>
       <c r="F91" s="52" t="s">
         <v>90</v>
       </c>
       <c r="G91" s="25"/>
     </row>
     <row r="92" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A92" s="60"/>
+      <c r="A92" s="63"/>
       <c r="B92" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C92" s="22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D92" s="22" t="s">
         <v>100</v>
@@ -5149,13 +5145,13 @@
       <c r="G93" s="24"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A94" s="59"/>
+      <c r="A94" s="62"/>
       <c r="B94" s="8"/>
       <c r="C94" s="41" t="s">
         <v>97</v>
       </c>
       <c r="D94" s="41" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E94" s="41" t="s">
         <v>90</v>
@@ -5166,15 +5162,15 @@
       <c r="G94" s="41"/>
     </row>
     <row r="95" spans="1:7" ht="250.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="60"/>
+      <c r="A95" s="63"/>
       <c r="B95" s="8" t="s">
         <v>65</v>
       </c>
       <c r="C95" s="21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D95" s="21" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="E95" s="21"/>
       <c r="F95" s="52" t="s">
@@ -5185,15 +5181,15 @@
       </c>
     </row>
     <row r="96" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A96" s="60"/>
+      <c r="A96" s="63"/>
       <c r="B96" s="8" t="s">
         <v>66</v>
       </c>
       <c r="C96" s="25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D96" s="25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E96" s="25"/>
       <c r="F96" s="52" t="s">
@@ -5202,15 +5198,15 @@
       <c r="G96" s="25"/>
     </row>
     <row r="97" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A97" s="60"/>
+      <c r="A97" s="63"/>
       <c r="B97" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C97" s="22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D97" s="25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E97" s="22"/>
       <c r="F97" s="52" t="s">
@@ -5236,40 +5232,40 @@
       <c r="A99" s="55"/>
       <c r="B99" s="8"/>
       <c r="C99" s="41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D99" s="41" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A100" s="55"/>
       <c r="B100" s="8"/>
       <c r="C100" s="21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D100" s="21" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A101" s="55"/>
       <c r="B101" s="8"/>
       <c r="C101" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D101" s="25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A102" s="55"/>
       <c r="B102" s="8"/>
       <c r="C102" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D102" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
@@ -5289,17 +5285,17 @@
         <v>103</v>
       </c>
       <c r="D104" s="41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="203" x14ac:dyDescent="0.35">
       <c r="A105" s="55"/>
       <c r="B105" s="8"/>
       <c r="C105" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D105" s="21" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
@@ -5309,7 +5305,7 @@
         <v>104</v>
       </c>
       <c r="D106" s="25" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -5319,7 +5315,7 @@
         <v>105</v>
       </c>
       <c r="D107" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
@@ -5343,7 +5339,7 @@
       <c r="A110" s="55"/>
       <c r="B110" s="8"/>
       <c r="C110" s="21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
@@ -5368,7 +5364,7 @@
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A114" s="59" t="s">
+      <c r="A114" s="62" t="s">
         <v>67</v>
       </c>
       <c r="B114" s="7" t="s">
@@ -5391,7 +5387,7 @@
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A115" s="59"/>
+      <c r="A115" s="62"/>
       <c r="B115" s="12"/>
       <c r="C115" s="42" t="s">
         <v>109</v>
@@ -5405,12 +5401,12 @@
       <c r="F115" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="G115" s="62" t="s">
-        <v>211</v>
+      <c r="G115" s="59" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="116" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A116" s="60"/>
+      <c r="A116" s="63"/>
       <c r="B116" s="8" t="s">
         <v>69</v>
       </c>
@@ -5429,17 +5425,17 @@
         <v>90</v>
       </c>
       <c r="G116" s="24" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="319" x14ac:dyDescent="0.35">
-      <c r="A117" s="60"/>
+      <c r="A117" s="63"/>
       <c r="B117" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C117" s="44" t="s">
         <v>194</v>
       </c>
-      <c r="C117" s="44" t="s">
-        <v>195</v>
-      </c>
       <c r="D117" s="44" t="s">
         <v>90</v>
       </c>
@@ -5449,17 +5445,17 @@
       <c r="F117" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="G117" s="63" t="s">
-        <v>213</v>
+      <c r="G117" s="60" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A118" s="60"/>
+      <c r="A118" s="63"/>
       <c r="B118" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C118" s="31" t="s">
-        <v>196</v>
+        <v>222</v>
       </c>
       <c r="D118" s="31" t="s">
         <v>90</v>
@@ -5471,11 +5467,11 @@
         <v>90</v>
       </c>
       <c r="G118" s="51" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A119" s="60"/>
+      <c r="A119" s="63"/>
       <c r="B119" s="5" t="str">
         <f>$B7</f>
         <v>#### Clearing:
@@ -5495,12 +5491,12 @@
       <c r="F119" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="G119" s="64" t="s">
-        <v>215</v>
+      <c r="G119" s="61" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A120" s="59" t="s">
+      <c r="A120" s="62" t="s">
         <v>70</v>
       </c>
       <c r="B120" s="11" t="s">
@@ -5513,7 +5509,7 @@
         <v>71</v>
       </c>
       <c r="E120" s="34" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F120" s="34" t="s">
         <v>71</v>
@@ -5523,13 +5519,13 @@
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A121" s="59"/>
+      <c r="A121" s="62"/>
       <c r="B121" s="13"/>
       <c r="C121" s="39" t="s">
         <v>90</v>
       </c>
       <c r="D121" s="39" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="E121" s="39" t="s">
         <v>110</v>
@@ -5539,7 +5535,7 @@
       </c>
     </row>
     <row r="122" spans="1:7" ht="237.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A122" s="59"/>
+      <c r="A122" s="62"/>
       <c r="B122" s="12" t="s">
         <v>72</v>
       </c>
@@ -5547,17 +5543,17 @@
         <v>90</v>
       </c>
       <c r="D122" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E122" s="21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F122" s="39" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="116" x14ac:dyDescent="0.35">
-      <c r="A123" s="59"/>
+      <c r="A123" s="62"/>
       <c r="B123" s="13" t="s">
         <v>73</v>
       </c>
@@ -5565,17 +5561,17 @@
         <v>90</v>
       </c>
       <c r="D123" s="25" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="E123" s="24" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="F123" s="39" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A124" s="59"/>
+      <c r="A124" s="62"/>
       <c r="B124" s="13" t="s">
         <v>47</v>
       </c>
@@ -5588,7 +5584,7 @@
       </c>
     </row>
     <row r="125" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A125" s="59"/>
+      <c r="A125" s="62"/>
       <c r="B125" s="13" t="s">
         <v>52</v>
       </c>
@@ -5601,7 +5597,7 @@
       </c>
     </row>
     <row r="126" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A126" s="59" t="s">
+      <c r="A126" s="62" t="s">
         <v>74</v>
       </c>
       <c r="B126" s="7" t="s">
@@ -5624,10 +5620,10 @@
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A127" s="59"/>
+      <c r="A127" s="62"/>
       <c r="B127" s="8"/>
       <c r="C127" s="41" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D127" s="41" t="s">
         <v>113</v>
@@ -5640,7 +5636,7 @@
       </c>
     </row>
     <row r="128" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A128" s="59"/>
+      <c r="A128" s="62"/>
       <c r="B128" s="8" t="s">
         <v>41</v>
       </c>
@@ -5658,49 +5654,49 @@
       </c>
     </row>
     <row r="129" spans="1:6" ht="388.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="59"/>
+      <c r="A129" s="62"/>
       <c r="B129" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="C129" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="C129" s="21" t="s">
+      <c r="D129" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="E129" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="F129" s="39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" ht="145" x14ac:dyDescent="0.35">
+      <c r="A130" s="62"/>
+      <c r="B130" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="D129" s="21" t="s">
-        <v>199</v>
-      </c>
-      <c r="E129" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="F129" s="39" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" ht="145" x14ac:dyDescent="0.35">
-      <c r="A130" s="59"/>
-      <c r="B130" s="8" t="s">
-        <v>191</v>
-      </c>
       <c r="C130" s="29" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="D130" s="29" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
     </row>
     <row r="131" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A131" s="59"/>
+      <c r="A131" s="62"/>
       <c r="B131" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C131" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D131" s="22" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="132" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A132" s="59"/>
+      <c r="A132" s="62"/>
       <c r="B132" s="13" t="s">
         <v>52</v>
       </c>
@@ -5712,13 +5708,13 @@
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A133" s="59"/>
+      <c r="A133" s="62"/>
       <c r="B133" s="8"/>
       <c r="C133" s="41" t="s">
         <v>112</v>
       </c>
       <c r="D133" s="41" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E133" s="39" t="s">
         <v>90</v>
@@ -5728,7 +5724,7 @@
       </c>
     </row>
     <row r="134" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A134" s="59"/>
+      <c r="A134" s="62"/>
       <c r="B134" s="8" t="s">
         <v>41</v>
       </c>
@@ -5746,15 +5742,15 @@
       </c>
     </row>
     <row r="135" spans="1:6" ht="290" x14ac:dyDescent="0.35">
-      <c r="A135" s="59"/>
+      <c r="A135" s="62"/>
       <c r="B135" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C135" s="21" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D135" s="21" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="E135" s="39" t="s">
         <v>90</v>
@@ -5764,31 +5760,31 @@
       </c>
     </row>
     <row r="136" spans="1:6" ht="145" x14ac:dyDescent="0.35">
-      <c r="A136" s="59"/>
+      <c r="A136" s="62"/>
       <c r="B136" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C136" s="29" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="D136" s="29" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
     </row>
     <row r="137" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A137" s="59"/>
+      <c r="A137" s="62"/>
       <c r="B137" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C137" s="22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D137" s="25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="138" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A138" s="59"/>
+      <c r="A138" s="62"/>
       <c r="B138" s="13" t="s">
         <v>52</v>
       </c>
@@ -5796,24 +5792,24 @@
         <v>102</v>
       </c>
       <c r="D138" s="24" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A139" s="59"/>
+      <c r="A139" s="62"/>
       <c r="B139" s="8"/>
       <c r="C139" s="41" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D139" s="41" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E139" s="52" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="140" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A140" s="59"/>
+      <c r="A140" s="62"/>
       <c r="B140" s="8"/>
       <c r="C140" s="31" t="s">
         <v>41</v>
@@ -5823,57 +5819,57 @@
       </c>
     </row>
     <row r="141" spans="1:6" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A141" s="59"/>
+      <c r="A141" s="62"/>
       <c r="B141" s="8"/>
       <c r="C141" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D141" s="21" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="142" spans="1:6" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A142" s="59"/>
+      <c r="A142" s="62"/>
       <c r="B142" s="8"/>
       <c r="C142" s="29" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="D142" s="29" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
     </row>
     <row r="143" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A143" s="59"/>
+      <c r="A143" s="62"/>
       <c r="B143" s="8"/>
       <c r="C143" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D143" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="144" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A144" s="59"/>
+      <c r="A144" s="62"/>
       <c r="B144" s="8"/>
       <c r="C144" s="24" t="s">
         <v>102</v>
       </c>
       <c r="D144" s="24" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A145" s="59"/>
+      <c r="A145" s="62"/>
       <c r="B145" s="8"/>
       <c r="C145" s="41" t="s">
         <v>114</v>
       </c>
       <c r="D145" s="41" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="146" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A146" s="59"/>
+      <c r="A146" s="62"/>
       <c r="B146" s="8"/>
       <c r="C146" s="31" t="s">
         <v>41</v>
@@ -5883,89 +5879,89 @@
       </c>
     </row>
     <row r="147" spans="1:7" ht="290" x14ac:dyDescent="0.35">
-      <c r="A147" s="59"/>
+      <c r="A147" s="62"/>
       <c r="B147" s="8"/>
       <c r="C147" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D147" s="21" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="148" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A148" s="59"/>
+      <c r="A148" s="62"/>
       <c r="B148" s="8"/>
       <c r="C148" s="29" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="D148" s="29" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
     </row>
     <row r="149" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A149" s="59"/>
+      <c r="A149" s="62"/>
       <c r="B149" s="8"/>
       <c r="C149" s="22" t="s">
         <v>105</v>
       </c>
       <c r="D149" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A150" s="59"/>
+      <c r="A150" s="62"/>
       <c r="B150" s="8"/>
       <c r="C150" s="24" t="s">
         <v>102</v>
       </c>
       <c r="D150" s="24" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A151" s="59"/>
+      <c r="A151" s="62"/>
       <c r="B151" s="8"/>
       <c r="C151" s="41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="152" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A152" s="59"/>
+      <c r="A152" s="62"/>
       <c r="B152" s="8"/>
       <c r="C152" s="31" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="153" spans="1:7" ht="275.5" x14ac:dyDescent="0.35">
-      <c r="A153" s="59"/>
+      <c r="A153" s="62"/>
       <c r="B153" s="8"/>
       <c r="C153" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="154" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A154" s="59"/>
+      <c r="A154" s="62"/>
       <c r="B154" s="8"/>
       <c r="C154" s="29" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
     </row>
     <row r="155" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A155" s="59"/>
+      <c r="A155" s="62"/>
       <c r="B155" s="8"/>
       <c r="C155" s="22" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="156" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A156" s="59"/>
+      <c r="A156" s="62"/>
       <c r="B156" s="8"/>
       <c r="C156" s="24" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="157" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A157" s="60" t="s">
+      <c r="A157" s="63" t="s">
         <v>76</v>
       </c>
       <c r="B157" s="7" t="s">
@@ -5988,7 +5984,7 @@
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A158" s="60"/>
+      <c r="A158" s="63"/>
       <c r="B158" s="8"/>
       <c r="C158" s="31" t="s">
         <v>90</v>
@@ -5997,14 +5993,14 @@
         <v>90</v>
       </c>
       <c r="E158" s="41" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F158" s="31" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="159" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A159" s="60"/>
+      <c r="A159" s="63"/>
       <c r="B159" s="8" t="s">
         <v>41</v>
       </c>
@@ -6022,35 +6018,35 @@
       </c>
     </row>
     <row r="160" spans="1:7" ht="332.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A160" s="60"/>
+      <c r="A160" s="63"/>
       <c r="B160" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C160" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="D160" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="E160" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="F160" s="31" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+      <c r="A161" s="63"/>
+      <c r="B161" s="8" t="s">
         <v>181</v>
-      </c>
-      <c r="C160" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="D160" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="E160" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="F160" s="31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="161" spans="1:7" ht="145" x14ac:dyDescent="0.35">
-      <c r="A161" s="60"/>
-      <c r="B161" s="8" t="s">
-        <v>182</v>
       </c>
       <c r="C161" s="29"/>
       <c r="E161" s="29" t="s">
-        <v>201</v>
+        <v>220</v>
       </c>
     </row>
     <row r="162" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A162" s="60"/>
+      <c r="A162" s="63"/>
       <c r="B162" s="15" t="s">
         <v>47</v>
       </c>
@@ -6060,7 +6056,7 @@
       </c>
     </row>
     <row r="163" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A163" s="60"/>
+      <c r="A163" s="63"/>
       <c r="B163" s="13" t="s">
         <v>52</v>
       </c>
@@ -6070,7 +6066,7 @@
       </c>
     </row>
     <row r="164" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A164" s="60" t="s">
+      <c r="A164" s="63" t="s">
         <v>78</v>
       </c>
       <c r="B164" s="7" t="s">
@@ -6093,7 +6089,7 @@
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A165" s="60"/>
+      <c r="A165" s="63"/>
       <c r="B165" s="8"/>
       <c r="C165" s="46"/>
       <c r="D165" s="41" t="s">
@@ -6103,7 +6099,7 @@
       <c r="F165" s="46"/>
     </row>
     <row r="166" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A166" s="60"/>
+      <c r="A166" s="63"/>
       <c r="B166" s="8" t="s">
         <v>41</v>
       </c>
@@ -6121,15 +6117,15 @@
       </c>
     </row>
     <row r="167" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A167" s="60"/>
+      <c r="A167" s="63"/>
       <c r="B167" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C167" s="29" t="s">
         <v>90</v>
       </c>
       <c r="D167" s="21" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E167" s="29" t="s">
         <v>90</v>
@@ -6139,17 +6135,17 @@
       </c>
     </row>
     <row r="168" spans="1:7" ht="145" x14ac:dyDescent="0.35">
-      <c r="A168" s="60"/>
+      <c r="A168" s="63"/>
       <c r="B168" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C168" s="29"/>
       <c r="D168" s="29" t="s">
-        <v>200</v>
+        <v>221</v>
       </c>
     </row>
     <row r="169" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A169" s="60"/>
+      <c r="A169" s="63"/>
       <c r="B169" s="15" t="s">
         <v>47</v>
       </c>
@@ -6159,7 +6155,7 @@
       </c>
     </row>
     <row r="170" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A170" s="60"/>
+      <c r="A170" s="63"/>
       <c r="B170" s="13" t="s">
         <v>52</v>
       </c>
@@ -6169,7 +6165,7 @@
       </c>
     </row>
     <row r="171" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A171" s="60" t="s">
+      <c r="A171" s="63" t="s">
         <v>80</v>
       </c>
       <c r="B171" s="7" t="s">
@@ -6192,7 +6188,7 @@
       </c>
     </row>
     <row r="172" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A172" s="60"/>
+      <c r="A172" s="63"/>
       <c r="B172" s="8" t="s">
         <v>41</v>
       </c>
@@ -6210,9 +6206,9 @@
       </c>
     </row>
     <row r="173" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A173" s="60"/>
+      <c r="A173" s="63"/>
       <c r="B173" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C173" s="29" t="s">
         <v>90</v>
@@ -6228,14 +6224,14 @@
       </c>
     </row>
     <row r="174" spans="1:7" ht="145" x14ac:dyDescent="0.35">
-      <c r="A174" s="60"/>
+      <c r="A174" s="63"/>
       <c r="B174" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C174" s="29"/>
     </row>
     <row r="175" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A175" s="60"/>
+      <c r="A175" s="63"/>
       <c r="B175" s="15" t="s">
         <v>47</v>
       </c>
@@ -6249,7 +6245,7 @@
       <c r="C176" s="29"/>
     </row>
     <row r="177" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A177" s="60" t="s">
+      <c r="A177" s="63" t="s">
         <v>82</v>
       </c>
       <c r="B177" s="7" t="s">
@@ -6272,7 +6268,7 @@
       </c>
     </row>
     <row r="178" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A178" s="60"/>
+      <c r="A178" s="63"/>
       <c r="B178" s="8" t="s">
         <v>41</v>
       </c>
@@ -6290,9 +6286,9 @@
       </c>
     </row>
     <row r="179" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A179" s="60"/>
+      <c r="A179" s="63"/>
       <c r="B179" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C179" s="52" t="s">
         <v>90</v>
@@ -6308,13 +6304,13 @@
       </c>
     </row>
     <row r="180" spans="1:7" ht="145" x14ac:dyDescent="0.35">
-      <c r="A180" s="60"/>
+      <c r="A180" s="63"/>
       <c r="B180" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="181" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A181" s="60"/>
+      <c r="A181" s="63"/>
       <c r="B181" s="8" t="s">
         <v>47</v>
       </c>
@@ -6323,7 +6319,7 @@
       </c>
     </row>
     <row r="182" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A182" s="60"/>
+      <c r="A182" s="63"/>
       <c r="B182" s="16" t="s">
         <v>52</v>
       </c>
@@ -6332,7 +6328,7 @@
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A183" s="60"/>
+      <c r="A183" s="63"/>
       <c r="C183" s="29"/>
     </row>
     <row r="184" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.35">
@@ -6458,6 +6454,16 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="A177:A183"/>
     <mergeCell ref="A59:A62"/>
@@ -6473,16 +6479,6 @@
     <mergeCell ref="A164:A170"/>
     <mergeCell ref="A50:A53"/>
     <mergeCell ref="A54:A58"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
Update documentation for the comments.
</commit_message>
<xml_diff>
--- a/testing/OperationKeyManagement+testcase.docs.xlsx
+++ b/testing/OperationKeyManagement+testcase.docs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venka\Documents\GitHub\Test2\OperationKeyManagement\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venka\MW_Testing\OKM_Final\OperationKeyManagement\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E1A881-151C-4DA0-ABCB-F647DE91BB60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D311A977-CCFB-4400-9EDB-7C3A5DDE472B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{8A4BF7CC-909B-4C1B-B59F-29AF2D960B3A}"/>
   </bookViews>
@@ -1220,15 +1220,6 @@
 - ApplicationLayerTopology server to operate</t>
   </si>
   <si>
-    <t>#### Testing:
-- POST ExecutionAndTraceLog/v1/list-records-of-flow with 
-   - IP, protocol and port from above
-   - operation-key from above
-   - DummyValue of x-correlator
-   - checking response 
-   - checking same record for containing DummyXCorrelator and application-name=applicationName from list retrieved from /v1/list-end-points-of-link, operation-name=update-operation-ket, trace-indicator=expected unique trace-indicator(values appened with unique numbers) and other attributes as expected.</t>
-  </si>
-  <si>
     <t>"#### Clearing:
 - not applicable"</t>
   </si>
@@ -1386,6 +1377,15 @@
    - attribute according to randomly chosen link-uuid from above
    -operation-key from above
    - all parameters with realistic values (incl. DummyXCorrelator)</t>
+  </si>
+  <si>
+    <t>#### Testing:
+- POST ExecutionAndTraceLog/v1/list-records-of-flow with 
+   - IP, protocol and port from above
+   - operation-key from above
+   - DummyValue of x-correlator
+   - checking response 
+   - checking same record for containing DummyXCorrelator and application-name=applicationName from list retrieved from /v1/list-end-points-of-link, operation-name=update-operation-key, trace-indicator=expected unique trace-indicator(values appended with unique numbers) and other attributes as expected.</t>
   </si>
 </sst>
 </file>
@@ -2182,10 +2182,10 @@
   <dimension ref="A1:G223"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B147" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="E117" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D150" sqref="D150"/>
+      <selection pane="bottomRight" activeCell="G118" sqref="G118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4203,7 +4203,7 @@
         <v>90</v>
       </c>
       <c r="F52" s="51" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G52" s="51"/>
     </row>
@@ -5170,7 +5170,7 @@
         <v>159</v>
       </c>
       <c r="D95" s="21" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E95" s="21"/>
       <c r="F95" s="52" t="s">
@@ -5245,7 +5245,7 @@
         <v>163</v>
       </c>
       <c r="D100" s="21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
@@ -5295,7 +5295,7 @@
         <v>162</v>
       </c>
       <c r="D105" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
@@ -5446,7 +5446,7 @@
         <v>90</v>
       </c>
       <c r="G117" s="60" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
@@ -5455,7 +5455,7 @@
         <v>187</v>
       </c>
       <c r="C118" s="31" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D118" s="31" t="s">
         <v>90</v>
@@ -5467,7 +5467,7 @@
         <v>90</v>
       </c>
       <c r="G118" s="51" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -5492,7 +5492,7 @@
         <v>90</v>
       </c>
       <c r="G119" s="61" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.35">
@@ -5561,10 +5561,10 @@
         <v>90</v>
       </c>
       <c r="D123" s="25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E123" s="24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F123" s="39" t="s">
         <v>90</v>
@@ -5677,10 +5677,10 @@
         <v>190</v>
       </c>
       <c r="C130" s="29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D130" s="29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="131" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
@@ -5750,7 +5750,7 @@
         <v>191</v>
       </c>
       <c r="D135" s="21" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E135" s="39" t="s">
         <v>90</v>
@@ -5765,10 +5765,10 @@
         <v>190</v>
       </c>
       <c r="C136" s="29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D136" s="29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="137" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
@@ -5825,17 +5825,17 @@
         <v>192</v>
       </c>
       <c r="D141" s="21" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="142" spans="1:6" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A142" s="62"/>
       <c r="B142" s="8"/>
       <c r="C142" s="29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D142" s="29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="143" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -5885,17 +5885,17 @@
         <v>178</v>
       </c>
       <c r="D147" s="21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="148" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A148" s="62"/>
       <c r="B148" s="8"/>
       <c r="C148" s="29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D148" s="29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="149" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -5943,7 +5943,7 @@
       <c r="A154" s="62"/>
       <c r="B154" s="8"/>
       <c r="C154" s="29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="155" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -6042,7 +6042,7 @@
       </c>
       <c r="C161" s="29"/>
       <c r="E161" s="29" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="162" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -6141,7 +6141,7 @@
       </c>
       <c r="C168" s="29"/>
       <c r="D168" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="169" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -6454,16 +6454,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="A177:A183"/>
     <mergeCell ref="A59:A62"/>
@@ -6479,6 +6469,16 @@
     <mergeCell ref="A164:A170"/>
     <mergeCell ref="A50:A53"/>
     <mergeCell ref="A54:A58"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
findings in test-suite Fixes #199
</commit_message>
<xml_diff>
--- a/testing/OperationKeyManagement+testcase.docs.xlsx
+++ b/testing/OperationKeyManagement+testcase.docs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venka\MW_Testing\OKM_Final\OperationKeyManagement\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IS00759329\Desktop\Telefonica\ApplicationPattern\ApplicationPattern_v2\OperationKeyManagement\OperationKeyManagement-4\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D311A977-CCFB-4400-9EDB-7C3A5DDE472B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2787F61F-36FF-461C-B86B-CE98932CB044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{8A4BF7CC-909B-4C1B-B59F-29AF2D960B3A}"/>
+    <workbookView xWindow="285" yWindow="270" windowWidth="20205" windowHeight="10650" xr2:uid="{8A4BF7CC-909B-4C1B-B59F-29AF2D960B3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Servicelayer" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="225">
   <si>
     <t>Testcases</t>
   </si>
@@ -1386,6 +1386,14 @@
    - DummyValue of x-correlator
    - checking response 
    - checking same record for containing DummyXCorrelator and application-name=applicationName from list retrieved from /v1/list-end-points-of-link, operation-name=update-operation-key, trace-indicator=expected unique trace-indicator(values appended with unique numbers) and other attributes as expected.</t>
+  </si>
+  <si>
+    <t>#### Clearing:
+- PUT initial newRelease/application-name
+- PUT initial newRelease/release-number
+- PUT initial newRelease/protocol
+- PUT initial newRelease/address
+- PUT initial newRelease/port</t>
   </si>
 </sst>
 </file>
@@ -2181,24 +2189,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6438CD8-A3F3-4ED1-9D84-D5D573F05C15}">
   <dimension ref="A1:G223"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="E117" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B117" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G118" sqref="G118"/>
+      <selection pane="bottomRight" activeCell="C120" sqref="C120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.54296875" style="58" customWidth="1"/>
-    <col min="2" max="2" width="70.7265625" style="2"/>
-    <col min="3" max="6" width="70.7265625" style="52"/>
-    <col min="7" max="7" width="70.7265625" style="52" customWidth="1"/>
-    <col min="8" max="40" width="9.1796875" style="52" customWidth="1"/>
-    <col min="41" max="16384" width="9.1796875" style="52"/>
+    <col min="1" max="1" width="35.5703125" style="58" customWidth="1"/>
+    <col min="2" max="2" width="70.7109375" style="2"/>
+    <col min="3" max="6" width="70.7109375" style="52"/>
+    <col min="7" max="7" width="70.7109375" style="52" customWidth="1"/>
+    <col min="8" max="40" width="9.140625" style="52" customWidth="1"/>
+    <col min="41" max="16384" width="9.140625" style="52"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
         <v>122</v>
       </c>
@@ -2209,7 +2217,7 @@
       <c r="F1" s="17"/>
       <c r="G1" s="17"/>
     </row>
-    <row r="2" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="54" t="s">
         <v>0</v>
       </c>
@@ -2221,7 +2229,7 @@
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
     </row>
-    <row r="3" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="54" t="s">
         <v>1</v>
       </c>
@@ -2244,7 +2252,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
         <v>3</v>
       </c>
@@ -2272,7 +2280,7 @@
         <v>## Is service idempotent?</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="225" x14ac:dyDescent="0.25">
       <c r="A5" s="62"/>
       <c r="B5" s="5" t="s">
         <v>5</v>
@@ -2351,7 +2359,7 @@
    - reasonable parameters</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="62"/>
       <c r="B6" s="5" t="s">
         <v>6</v>
@@ -2386,7 +2394,7 @@
 </v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="62"/>
       <c r="B7" s="6" t="s">
         <v>7</v>
@@ -2415,7 +2423,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="62" t="s">
         <v>8</v>
       </c>
@@ -2443,7 +2451,7 @@
         <v>## Get parameters checked for completeness?</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="255" x14ac:dyDescent="0.25">
       <c r="A9" s="62"/>
       <c r="B9" s="8" t="s">
         <v>10</v>
@@ -2522,7 +2530,7 @@
     -  BUT one randomly chosen parameter (user, originator, x-correlator, trace-indicator or customer-journey) missing (not empty string!)</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="62"/>
       <c r="B10" s="8" t="s">
         <v>11</v>
@@ -2553,7 +2561,7 @@
 - checking for ResponseCode == 400</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="62"/>
       <c r="B11" s="6" t="str">
         <f>$B7</f>
@@ -2584,7 +2592,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="62" t="s">
         <v>12</v>
       </c>
@@ -2612,7 +2620,7 @@
         <v>## Gets originator checked for compliance with specification?</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="255" x14ac:dyDescent="0.25">
       <c r="A13" s="62"/>
       <c r="B13" s="8" t="s">
         <v>14</v>
@@ -2692,7 +2700,7 @@
           1.  originator set to be a string of 0, 1 or 2 (random) letters length (too short).</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="62"/>
       <c r="B14" s="8" t="s">
         <v>15</v>
@@ -2723,7 +2731,7 @@
 - checking for ResponseCode==400</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="62"/>
       <c r="B15" s="6" t="str">
         <f>$B7</f>
@@ -2754,7 +2762,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="62" t="s">
         <v>16</v>
       </c>
@@ -2782,7 +2790,7 @@
         <v>## Gets x-correlator checked for complying the pattern?</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="240" x14ac:dyDescent="0.25">
       <c r="A17" s="62"/>
       <c r="B17" s="8" t="s">
         <v>18</v>
@@ -2860,7 +2868,7 @@
    - reasonable parameters, BUT dummyXCorrelators differing from the pattern in various ways (e.g. empty string)</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="62"/>
       <c r="B18" s="8" t="s">
         <v>15</v>
@@ -2891,7 +2899,7 @@
 - checking for ResponseCode==400</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="62"/>
       <c r="B19" s="6" t="str">
         <f>$B7</f>
@@ -2922,7 +2930,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="62" t="s">
         <v>19</v>
       </c>
@@ -2950,7 +2958,7 @@
         <v>## Gets trace-indicator checked for complying the pattern?</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="240" x14ac:dyDescent="0.25">
       <c r="A21" s="62"/>
       <c r="B21" s="8" t="s">
         <v>21</v>
@@ -3028,7 +3036,7 @@
    - reasonable parameters, BUT dummyTraceIndicator differing from the pattern in various ways (e.g. empty string)</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="62"/>
       <c r="B22" s="8" t="s">
         <v>15</v>
@@ -3059,7 +3067,7 @@
 - checking for ResponseCode==400</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="62"/>
       <c r="B23" s="6" t="str">
         <f>$B7</f>
@@ -3090,7 +3098,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="62" t="s">
         <v>22</v>
       </c>
@@ -3118,7 +3126,7 @@
         <v>## Gets security key checked for availability?</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="210" x14ac:dyDescent="0.25">
       <c r="A25" s="62"/>
       <c r="B25" s="8" t="s">
         <v>24</v>
@@ -3181,7 +3189,7 @@
     - BUT operationKey parameter missing (does not mean empty string)</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="62"/>
       <c r="B26" s="8" t="s">
         <v>25</v>
@@ -3212,7 +3220,7 @@
 - checking for ResponseCode==401</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="62"/>
       <c r="B27" s="6" t="str">
         <f>$B7</f>
@@ -3243,7 +3251,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="62" t="s">
         <v>26</v>
       </c>
@@ -3271,7 +3279,7 @@
         <v>## Gets security key checked for correctness?</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="210" x14ac:dyDescent="0.25">
       <c r="A29" s="62"/>
       <c r="B29" s="8" t="s">
         <v>28</v>
@@ -3334,7 +3342,7 @@
      - BUT operationKey parameter with random dummy value</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="62"/>
       <c r="B30" s="8" t="s">
         <v>25</v>
@@ -3365,7 +3373,7 @@
 - checking for ResponseCode==401</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="62"/>
       <c r="B31" s="6" t="str">
         <f>$B7</f>
@@ -3396,7 +3404,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="62" t="s">
         <v>29</v>
       </c>
@@ -3424,7 +3432,7 @@
         <v>## Contains response complete set of headers?</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="225" x14ac:dyDescent="0.25">
       <c r="A33" s="62"/>
       <c r="B33" s="8" t="s">
         <v>31</v>
@@ -3482,7 +3490,7 @@
    - reasonable parameters</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="62"/>
       <c r="B34" s="8" t="s">
         <v>32</v>
@@ -3509,7 +3517,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="62"/>
       <c r="B35" s="6" t="str">
         <f>$B7</f>
@@ -3540,7 +3548,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="62" t="s">
         <v>33</v>
       </c>
@@ -3568,7 +3576,7 @@
         <v>## Is the initial x-correlator ín the response?</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" ht="225" x14ac:dyDescent="0.25">
       <c r="A37" s="62"/>
       <c r="B37" s="8" t="s">
         <v>31</v>
@@ -3626,7 +3634,7 @@
    - reasonable parameters</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="62"/>
       <c r="B38" s="8" t="s">
         <v>35</v>
@@ -3656,7 +3664,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="62"/>
       <c r="B39" s="6" t="str">
         <f>$B7</f>
@@ -3687,7 +3695,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="62" t="s">
         <v>36</v>
       </c>
@@ -3715,7 +3723,7 @@
         <v>## Is the correct life-cycle-state ín the response?</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" ht="225" x14ac:dyDescent="0.25">
       <c r="A41" s="63"/>
       <c r="B41" s="8" t="s">
         <v>31</v>
@@ -3773,7 +3781,7 @@
    - reasonable parameters</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="63"/>
       <c r="B42" s="8" t="s">
         <v>38</v>
@@ -3819,7 +3827,7 @@
 - checking for response headers containing life-cycle-state is equal to the value as present in the control-construct for /v1/regard-updated-link/configuration/life-cycle-state</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="63"/>
       <c r="B43" s="6" t="str">
         <f>$B7</f>
@@ -3850,7 +3858,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="62" t="s">
         <v>39</v>
       </c>
@@ -3873,7 +3881,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="63"/>
       <c r="B45" s="8" t="s">
         <v>41</v>
@@ -3894,7 +3902,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" ht="300" x14ac:dyDescent="0.25">
       <c r="A46" s="63"/>
       <c r="B46" s="8" t="s">
         <v>185</v>
@@ -4005,7 +4013,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A47" s="63"/>
       <c r="B47" s="8" t="s">
         <v>186</v>
@@ -4091,7 +4099,7 @@
    - checking same record for containing DummyXCorrelator &amp;DummyTraceIndicator</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="63"/>
       <c r="B48" s="9" t="str">
         <f>$B7</f>
@@ -4122,7 +4130,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="56" t="s">
         <v>42</v>
       </c>
@@ -4133,7 +4141,7 @@
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
     </row>
-    <row r="50" spans="1:7" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A50" s="64" t="s">
         <v>43</v>
       </c>
@@ -4156,7 +4164,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A51" s="62"/>
       <c r="B51" s="12" t="s">
         <v>45</v>
@@ -4188,7 +4196,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="171" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" ht="171" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="62"/>
       <c r="B52" s="13" t="s">
         <v>46</v>
@@ -4207,7 +4215,7 @@
       </c>
       <c r="G52" s="51"/>
     </row>
-    <row r="53" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="62"/>
       <c r="B53" s="14" t="s">
         <v>47</v>
@@ -4228,7 +4236,7 @@
       </c>
       <c r="G53" s="37"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="63" t="s">
         <v>48</v>
       </c>
@@ -4251,7 +4259,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="174" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A55" s="63"/>
       <c r="B55" s="12" t="s">
         <v>50</v>
@@ -4293,7 +4301,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" s="63"/>
       <c r="B56" s="13" t="s">
         <v>51</v>
@@ -4314,7 +4322,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="63"/>
       <c r="B57" s="14" t="s">
         <v>47</v>
@@ -4335,7 +4343,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="63"/>
       <c r="B58" s="13" t="s">
         <v>52</v>
@@ -4354,7 +4362,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="62" t="s">
         <v>53</v>
       </c>
@@ -4382,7 +4390,7 @@
         <v>## Gets lifeCycleState propagated?</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" ht="240" x14ac:dyDescent="0.25">
       <c r="A60" s="63"/>
       <c r="B60" s="8" t="s">
         <v>55</v>
@@ -4467,7 +4475,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="63"/>
       <c r="B61" s="8" t="s">
         <v>56</v>
@@ -4488,7 +4496,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="63"/>
       <c r="B62" s="15" t="s">
         <v>57</v>
@@ -4509,7 +4517,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="62" t="s">
         <v>58</v>
       </c>
@@ -4537,7 +4545,7 @@
         <v>## Get attributes checked for completeness?</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" ht="255" x14ac:dyDescent="0.25">
       <c r="A64" s="62"/>
       <c r="B64" s="8" t="s">
         <v>60</v>
@@ -4588,7 +4596,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="62"/>
       <c r="B65" s="8" t="s">
         <v>61</v>
@@ -4617,7 +4625,7 @@
 - checking for ResponseCode==400</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="62"/>
       <c r="B66" s="15" t="s">
         <v>47</v>
@@ -4646,7 +4654,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="62" t="s">
         <v>133</v>
       </c>
@@ -4674,7 +4682,7 @@
         <v>## Get each attributes checked for correctness?</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="62"/>
       <c r="B68" s="8"/>
       <c r="C68" s="41" t="s">
@@ -4693,7 +4701,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" ht="225" x14ac:dyDescent="0.25">
       <c r="A69" s="62"/>
       <c r="B69" s="8"/>
       <c r="C69" s="21" t="s">
@@ -4732,7 +4740,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="62"/>
       <c r="B70" s="8"/>
       <c r="C70" s="25" t="str">
@@ -4750,7 +4758,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="62"/>
       <c r="B71" s="8"/>
       <c r="C71" s="22" t="str">
@@ -4774,7 +4782,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="62"/>
       <c r="B72" s="8"/>
       <c r="C72" s="41" t="s">
@@ -4787,7 +4795,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" ht="240" x14ac:dyDescent="0.25">
       <c r="A73" s="62"/>
       <c r="B73" s="8"/>
       <c r="C73" s="21" t="s">
@@ -4814,7 +4822,7 @@
       </c>
       <c r="G73" s="21"/>
     </row>
-    <row r="74" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="62"/>
       <c r="B74" s="8"/>
       <c r="C74" s="25" t="str">
@@ -4829,7 +4837,7 @@
       </c>
       <c r="G74" s="25"/>
     </row>
-    <row r="75" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="62"/>
       <c r="B75" s="8"/>
       <c r="C75" s="50" t="str">
@@ -4844,7 +4852,7 @@
       </c>
       <c r="G75" s="22"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="62"/>
       <c r="B76" s="8"/>
       <c r="C76" s="41" t="s">
@@ -4854,7 +4862,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" ht="240" x14ac:dyDescent="0.25">
       <c r="A77" s="62"/>
       <c r="B77" s="8"/>
       <c r="C77" s="21" t="s">
@@ -4880,7 +4888,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="62"/>
       <c r="B78" s="8"/>
       <c r="C78" s="25" t="str">
@@ -4894,7 +4902,7 @@
 - checking for ResponseCode==400</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="62"/>
       <c r="B79" s="8"/>
       <c r="C79" s="22" t="str">
@@ -4908,7 +4916,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="62"/>
       <c r="B80" s="8"/>
       <c r="C80" s="41" t="s">
@@ -4918,7 +4926,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" ht="255" x14ac:dyDescent="0.25">
       <c r="A81" s="62"/>
       <c r="B81" s="8"/>
       <c r="C81" s="21" t="s">
@@ -4944,7 +4952,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="62"/>
       <c r="B82" s="8"/>
       <c r="C82" s="25" t="str">
@@ -4958,7 +4966,7 @@
 - checking for ResponseCode==400</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="62"/>
       <c r="B83" s="8"/>
       <c r="C83" s="22" t="str">
@@ -4972,7 +4980,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="62"/>
       <c r="B84" s="8"/>
       <c r="C84" s="22"/>
@@ -4980,7 +4988,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A85" s="62"/>
       <c r="B85" s="8"/>
       <c r="C85" s="22"/>
@@ -5004,7 +5012,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="62"/>
       <c r="B86" s="8"/>
       <c r="C86" s="22"/>
@@ -5014,7 +5022,7 @@
 - checking for ResponseCode==400</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="62"/>
       <c r="B87" s="8"/>
       <c r="C87" s="22"/>
@@ -5024,7 +5032,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="62" t="s">
         <v>63</v>
       </c>
@@ -5052,7 +5060,7 @@
         <v>## Get each attributes checked if getting correctly updated?</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="62"/>
       <c r="B89" s="8"/>
       <c r="C89" s="41" t="s">
@@ -5069,7 +5077,7 @@
       </c>
       <c r="G89" s="41"/>
     </row>
-    <row r="90" spans="1:7" ht="303" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" ht="303" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="63"/>
       <c r="B90" s="8" t="s">
         <v>65</v>
@@ -5090,7 +5098,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="63"/>
       <c r="B91" s="8" t="s">
         <v>66</v>
@@ -5109,7 +5117,7 @@
       </c>
       <c r="G91" s="25"/>
     </row>
-    <row r="92" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A92" s="63"/>
       <c r="B92" s="8" t="s">
         <v>47</v>
@@ -5128,7 +5136,7 @@
       </c>
       <c r="G92" s="22"/>
     </row>
-    <row r="93" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A93" s="55"/>
       <c r="B93" s="13" t="s">
         <v>52</v>
@@ -5144,7 +5152,7 @@
       </c>
       <c r="G93" s="24"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="62"/>
       <c r="B94" s="8"/>
       <c r="C94" s="41" t="s">
@@ -5161,7 +5169,7 @@
       </c>
       <c r="G94" s="41"/>
     </row>
-    <row r="95" spans="1:7" ht="250.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" ht="250.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="63"/>
       <c r="B95" s="8" t="s">
         <v>65</v>
@@ -5180,7 +5188,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A96" s="63"/>
       <c r="B96" s="8" t="s">
         <v>66</v>
@@ -5197,7 +5205,7 @@
       </c>
       <c r="G96" s="25"/>
     </row>
-    <row r="97" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A97" s="63"/>
       <c r="B97" s="8" t="s">
         <v>47</v>
@@ -5214,7 +5222,7 @@
       </c>
       <c r="G97" s="22"/>
     </row>
-    <row r="98" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A98" s="55"/>
       <c r="B98" s="13" t="s">
         <v>52</v>
@@ -5228,7 +5236,7 @@
       <c r="E98" s="24"/>
       <c r="G98" s="24"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="55"/>
       <c r="B99" s="8"/>
       <c r="C99" s="41" t="s">
@@ -5238,7 +5246,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" ht="225" x14ac:dyDescent="0.25">
       <c r="A100" s="55"/>
       <c r="B100" s="8"/>
       <c r="C100" s="21" t="s">
@@ -5248,7 +5256,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A101" s="55"/>
       <c r="B101" s="8"/>
       <c r="C101" s="25" t="s">
@@ -5258,7 +5266,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="55"/>
       <c r="B102" s="8"/>
       <c r="C102" s="22" t="s">
@@ -5268,7 +5276,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A103" s="55"/>
       <c r="B103" s="8"/>
       <c r="C103" s="24" t="s">
@@ -5278,7 +5286,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="55"/>
       <c r="B104" s="8"/>
       <c r="C104" s="41" t="s">
@@ -5288,7 +5296,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" ht="240" x14ac:dyDescent="0.25">
       <c r="A105" s="55"/>
       <c r="B105" s="8"/>
       <c r="C105" s="21" t="s">
@@ -5298,7 +5306,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A106" s="55"/>
       <c r="B106" s="8"/>
       <c r="C106" s="25" t="s">
@@ -5308,7 +5316,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="55"/>
       <c r="B107" s="8"/>
       <c r="C107" s="22" t="s">
@@ -5318,7 +5326,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A108" s="55"/>
       <c r="B108" s="8"/>
       <c r="C108" s="24" t="s">
@@ -5328,42 +5336,42 @@
         <v>102</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="55"/>
       <c r="B109" s="8"/>
       <c r="C109" s="41" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" ht="240" x14ac:dyDescent="0.25">
       <c r="A110" s="55"/>
       <c r="B110" s="8"/>
       <c r="C110" s="21" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A111" s="55"/>
       <c r="B111" s="8"/>
       <c r="C111" s="25" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="55"/>
       <c r="B112" s="8"/>
       <c r="C112" s="22" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A113" s="55"/>
       <c r="B113" s="8"/>
       <c r="C113" s="24" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="62" t="s">
         <v>67</v>
       </c>
@@ -5386,7 +5394,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="62"/>
       <c r="B115" s="12"/>
       <c r="C115" s="42" t="s">
@@ -5405,7 +5413,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" s="63"/>
       <c r="B116" s="8" t="s">
         <v>69</v>
@@ -5428,7 +5436,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="319" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:7" ht="375" x14ac:dyDescent="0.25">
       <c r="A117" s="63"/>
       <c r="B117" s="8" t="s">
         <v>193</v>
@@ -5449,7 +5457,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A118" s="63"/>
       <c r="B118" s="8" t="s">
         <v>187</v>
@@ -5470,17 +5478,15 @@
         <v>223</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A119" s="63"/>
       <c r="B119" s="5" t="str">
         <f>$B7</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
-      <c r="C119" s="45" t="str">
-        <f>$B7</f>
-        <v>#### Clearing:
-- not applicable</v>
+      <c r="C119" s="45" t="s">
+        <v>224</v>
       </c>
       <c r="D119" s="45" t="s">
         <v>90</v>
@@ -5495,7 +5501,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="62" t="s">
         <v>70</v>
       </c>
@@ -5518,7 +5524,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="62"/>
       <c r="B121" s="13"/>
       <c r="C121" s="39" t="s">
@@ -5534,7 +5540,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="237.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:7" ht="237.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="62"/>
       <c r="B122" s="12" t="s">
         <v>72</v>
@@ -5552,7 +5558,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A123" s="62"/>
       <c r="B123" s="13" t="s">
         <v>73</v>
@@ -5570,7 +5576,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A124" s="62"/>
       <c r="B124" s="13" t="s">
         <v>47</v>
@@ -5583,7 +5589,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A125" s="62"/>
       <c r="B125" s="13" t="s">
         <v>52</v>
@@ -5596,7 +5602,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="62" t="s">
         <v>74</v>
       </c>
@@ -5619,7 +5625,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="62"/>
       <c r="B127" s="8"/>
       <c r="C127" s="41" t="s">
@@ -5635,7 +5641,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="62"/>
       <c r="B128" s="8" t="s">
         <v>41</v>
@@ -5653,7 +5659,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="388.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:6" ht="388.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="62"/>
       <c r="B129" s="8" t="s">
         <v>188</v>
@@ -5671,7 +5677,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="145" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A130" s="62"/>
       <c r="B130" s="8" t="s">
         <v>190</v>
@@ -5683,7 +5689,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A131" s="62"/>
       <c r="B131" s="8" t="s">
         <v>47</v>
@@ -5695,7 +5701,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A132" s="62"/>
       <c r="B132" s="13" t="s">
         <v>52</v>
@@ -5707,7 +5713,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="62"/>
       <c r="B133" s="8"/>
       <c r="C133" s="41" t="s">
@@ -5723,7 +5729,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="62"/>
       <c r="B134" s="8" t="s">
         <v>41</v>
@@ -5741,7 +5747,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="290" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:6" ht="345" x14ac:dyDescent="0.25">
       <c r="A135" s="62"/>
       <c r="B135" s="8" t="s">
         <v>188</v>
@@ -5759,7 +5765,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="145" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A136" s="62"/>
       <c r="B136" s="8" t="s">
         <v>190</v>
@@ -5771,7 +5777,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A137" s="62"/>
       <c r="B137" s="8" t="s">
         <v>47</v>
@@ -5783,7 +5789,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A138" s="62"/>
       <c r="B138" s="13" t="s">
         <v>52</v>
@@ -5795,7 +5801,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="62"/>
       <c r="B139" s="8"/>
       <c r="C139" s="41" t="s">
@@ -5808,7 +5814,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A140" s="62"/>
       <c r="B140" s="8"/>
       <c r="C140" s="31" t="s">
@@ -5818,7 +5824,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:6" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="62"/>
       <c r="B141" s="8"/>
       <c r="C141" s="21" t="s">
@@ -5828,7 +5834,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A142" s="62"/>
       <c r="B142" s="8"/>
       <c r="C142" s="29" t="s">
@@ -5838,7 +5844,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="143" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="62"/>
       <c r="B143" s="8"/>
       <c r="C143" s="22" t="s">
@@ -5848,7 +5854,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A144" s="62"/>
       <c r="B144" s="8"/>
       <c r="C144" s="24" t="s">
@@ -5858,7 +5864,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="62"/>
       <c r="B145" s="8"/>
       <c r="C145" s="41" t="s">
@@ -5868,7 +5874,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="62"/>
       <c r="B146" s="8"/>
       <c r="C146" s="31" t="s">
@@ -5878,7 +5884,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="290" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:7" ht="360" x14ac:dyDescent="0.25">
       <c r="A147" s="62"/>
       <c r="B147" s="8"/>
       <c r="C147" s="21" t="s">
@@ -5888,7 +5894,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A148" s="62"/>
       <c r="B148" s="8"/>
       <c r="C148" s="29" t="s">
@@ -5898,7 +5904,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="62"/>
       <c r="B149" s="8"/>
       <c r="C149" s="22" t="s">
@@ -5908,7 +5914,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A150" s="62"/>
       <c r="B150" s="8"/>
       <c r="C150" s="24" t="s">
@@ -5918,49 +5924,49 @@
         <v>102</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="62"/>
       <c r="B151" s="8"/>
       <c r="C151" s="41" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="62"/>
       <c r="B152" s="8"/>
       <c r="C152" s="31" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:7" ht="360" x14ac:dyDescent="0.25">
       <c r="A153" s="62"/>
       <c r="B153" s="8"/>
       <c r="C153" s="21" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="154" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A154" s="62"/>
       <c r="B154" s="8"/>
       <c r="C154" s="29" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" s="62"/>
       <c r="B155" s="8"/>
       <c r="C155" s="22" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A156" s="62"/>
       <c r="B156" s="8"/>
       <c r="C156" s="24" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="63" t="s">
         <v>76</v>
       </c>
@@ -5983,7 +5989,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="63"/>
       <c r="B158" s="8"/>
       <c r="C158" s="31" t="s">
@@ -5999,7 +6005,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="63"/>
       <c r="B159" s="8" t="s">
         <v>41</v>
@@ -6017,7 +6023,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="332.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:7" ht="332.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="63"/>
       <c r="B160" s="8" t="s">
         <v>180</v>
@@ -6035,7 +6041,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A161" s="63"/>
       <c r="B161" s="8" t="s">
         <v>181</v>
@@ -6045,7 +6051,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="63"/>
       <c r="B162" s="15" t="s">
         <v>47</v>
@@ -6055,7 +6061,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A163" s="63"/>
       <c r="B163" s="13" t="s">
         <v>52</v>
@@ -6065,7 +6071,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="63" t="s">
         <v>78</v>
       </c>
@@ -6088,7 +6094,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="63"/>
       <c r="B165" s="8"/>
       <c r="C165" s="46"/>
@@ -6098,7 +6104,7 @@
       <c r="E165" s="46"/>
       <c r="F165" s="46"/>
     </row>
-    <row r="166" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="63"/>
       <c r="B166" s="8" t="s">
         <v>41</v>
@@ -6116,7 +6122,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:7" ht="240" x14ac:dyDescent="0.25">
       <c r="A167" s="63"/>
       <c r="B167" s="8" t="s">
         <v>180</v>
@@ -6134,7 +6140,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A168" s="63"/>
       <c r="B168" s="8" t="s">
         <v>182</v>
@@ -6144,7 +6150,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A169" s="63"/>
       <c r="B169" s="15" t="s">
         <v>47</v>
@@ -6154,7 +6160,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A170" s="63"/>
       <c r="B170" s="13" t="s">
         <v>52</v>
@@ -6164,7 +6170,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" s="63" t="s">
         <v>80</v>
       </c>
@@ -6187,7 +6193,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" s="63"/>
       <c r="B172" s="8" t="s">
         <v>41</v>
@@ -6205,7 +6211,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A173" s="63"/>
       <c r="B173" s="8" t="s">
         <v>180</v>
@@ -6223,28 +6229,28 @@
         <v>90</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A174" s="63"/>
       <c r="B174" s="8" t="s">
         <v>183</v>
       </c>
       <c r="C174" s="29"/>
     </row>
-    <row r="175" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A175" s="63"/>
       <c r="B175" s="15" t="s">
         <v>47</v>
       </c>
       <c r="C175" s="29"/>
     </row>
-    <row r="176" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" s="55"/>
       <c r="B176" s="13" t="s">
         <v>52</v>
       </c>
       <c r="C176" s="29"/>
     </row>
-    <row r="177" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="63" t="s">
         <v>82</v>
       </c>
@@ -6267,7 +6273,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="178" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A178" s="63"/>
       <c r="B178" s="8" t="s">
         <v>41</v>
@@ -6285,7 +6291,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="179" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A179" s="63"/>
       <c r="B179" s="8" t="s">
         <v>180</v>
@@ -6303,13 +6309,13 @@
         <v>90</v>
       </c>
     </row>
-    <row r="180" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A180" s="63"/>
       <c r="B180" s="8" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="181" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A181" s="63"/>
       <c r="B181" s="8" t="s">
         <v>47</v>
@@ -6318,7 +6324,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="182" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" s="63"/>
       <c r="B182" s="16" t="s">
         <v>52</v>
@@ -6327,133 +6333,143 @@
         <v>90</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="63"/>
       <c r="C183" s="29"/>
     </row>
-    <row r="184" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A184" s="57"/>
       <c r="C184" s="49"/>
     </row>
-    <row r="185" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A185" s="57"/>
     </row>
-    <row r="186" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A186" s="57"/>
     </row>
-    <row r="187" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A187" s="57"/>
     </row>
-    <row r="188" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A188" s="57"/>
     </row>
-    <row r="189" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A189" s="57"/>
     </row>
-    <row r="190" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A190" s="57"/>
     </row>
-    <row r="191" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="57"/>
     </row>
-    <row r="192" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A192" s="57"/>
     </row>
-    <row r="193" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A193" s="57"/>
     </row>
-    <row r="194" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A194" s="57"/>
     </row>
-    <row r="195" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A195" s="57"/>
     </row>
-    <row r="196" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A196" s="57"/>
     </row>
-    <row r="197" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A197" s="57"/>
     </row>
-    <row r="198" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198" s="57"/>
     </row>
-    <row r="199" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A199" s="57"/>
     </row>
-    <row r="200" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A200" s="57"/>
     </row>
-    <row r="201" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A201" s="57"/>
     </row>
-    <row r="202" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A202" s="57"/>
     </row>
-    <row r="203" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A203" s="57"/>
     </row>
-    <row r="204" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A204" s="57"/>
     </row>
-    <row r="205" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A205" s="57"/>
     </row>
-    <row r="206" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A206" s="57"/>
     </row>
-    <row r="207" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A207" s="57"/>
     </row>
-    <row r="208" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A208" s="57"/>
     </row>
-    <row r="209" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A209" s="57"/>
     </row>
-    <row r="210" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A210" s="57"/>
     </row>
-    <row r="211" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A211" s="57"/>
     </row>
-    <row r="212" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A212" s="57"/>
     </row>
-    <row r="213" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A213" s="57"/>
     </row>
-    <row r="214" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A214" s="57"/>
     </row>
-    <row r="215" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A215" s="57"/>
     </row>
-    <row r="216" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A216" s="57"/>
     </row>
-    <row r="217" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A217" s="57"/>
     </row>
-    <row r="218" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A218" s="57"/>
     </row>
-    <row r="219" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A219" s="57"/>
     </row>
-    <row r="220" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A220" s="57"/>
     </row>
-    <row r="221" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A221" s="57"/>
     </row>
-    <row r="222" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A222" s="57"/>
     </row>
-    <row r="223" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A223" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="A177:A183"/>
     <mergeCell ref="A59:A62"/>
@@ -6469,16 +6485,6 @@
     <mergeCell ref="A164:A170"/>
     <mergeCell ref="A50:A53"/>
     <mergeCell ref="A54:A58"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>